<commit_message>
update eme workflow related functions
</commit_message>
<xml_diff>
--- a/sitedb/smallcell data/milestone update table.xlsx
+++ b/sitedb/smallcell data/milestone update table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\005 VHA Macro site workflow\Django-Workflow\sitedb\smallcell data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\018 MongoDB\03 withmysql\VHA RAN Refresh\Django-Workflow\sitedb\smallcell data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0C1190-CBE9-4827-B922-A01B296CA9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50F3690-E889-46FA-B962-DE515CC3E4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6645" windowWidth="29040" windowHeight="15840" xr2:uid="{BA6B08D2-2D56-45E4-9B2D-1CBEB3F086CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA6B08D2-2D56-45E4-9B2D-1CBEB3F086CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="83">
   <si>
     <t>Site ID</t>
   </si>
@@ -252,9 +252,6 @@
     <t>activation_cr</t>
   </si>
   <si>
-    <t>emeg_check</t>
-  </si>
-  <si>
     <t>cell_activation</t>
   </si>
   <si>
@@ -268,6 +265,15 @@
   </si>
   <si>
     <t>dsa7_upload</t>
+  </si>
+  <si>
+    <t>form_b_ezone_letter</t>
+  </si>
+  <si>
+    <t>rfnsa_eme_ready</t>
+  </si>
+  <si>
+    <t>emeg_order</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1C2277-610E-4BB7-B1D6-1DA723A183E9}">
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AC49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -683,14 +689,15 @@
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,25 +762,31 @@
         <v>74</v>
       </c>
       <c r="V1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" t="s">
-        <v>80</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -855,8 +868,14 @@
       <c r="AA2" t="s">
         <v>22</v>
       </c>
+      <c r="AB2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -938,8 +957,14 @@
       <c r="AA3" t="s">
         <v>22</v>
       </c>
+      <c r="AB3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1021,8 +1046,14 @@
       <c r="AA4" t="s">
         <v>22</v>
       </c>
+      <c r="AB4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1104,8 +1135,14 @@
       <c r="AA5" t="s">
         <v>22</v>
       </c>
+      <c r="AB5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1187,8 +1224,14 @@
       <c r="AA6" t="s">
         <v>22</v>
       </c>
+      <c r="AB6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1270,8 +1313,14 @@
       <c r="AA7" t="s">
         <v>22</v>
       </c>
+      <c r="AB7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1353,8 +1402,14 @@
       <c r="AA8" t="s">
         <v>22</v>
       </c>
+      <c r="AB8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1436,8 +1491,14 @@
       <c r="AA9" t="s">
         <v>22</v>
       </c>
+      <c r="AB9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1519,8 +1580,14 @@
       <c r="AA10" t="s">
         <v>22</v>
       </c>
+      <c r="AB10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1602,8 +1669,14 @@
       <c r="AA11" t="s">
         <v>22</v>
       </c>
+      <c r="AB11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1685,8 +1758,14 @@
       <c r="AA12" t="s">
         <v>22</v>
       </c>
+      <c r="AB12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1768,8 +1847,14 @@
       <c r="AA13" t="s">
         <v>22</v>
       </c>
+      <c r="AB13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1851,8 +1936,14 @@
       <c r="AA14" t="s">
         <v>22</v>
       </c>
+      <c r="AB14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1934,8 +2025,14 @@
       <c r="AA15" t="s">
         <v>22</v>
       </c>
+      <c r="AB15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -2017,8 +2114,14 @@
       <c r="AA16" t="s">
         <v>22</v>
       </c>
+      <c r="AB16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -2086,10 +2189,10 @@
         <v>21</v>
       </c>
       <c r="W17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y17" t="s">
         <v>22</v>
@@ -2100,8 +2203,14 @@
       <c r="AA17" t="s">
         <v>22</v>
       </c>
+      <c r="AB17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -2172,10 +2281,10 @@
         <v>21</v>
       </c>
       <c r="X18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z18" t="s">
         <v>22</v>
@@ -2183,8 +2292,14 @@
       <c r="AA18" t="s">
         <v>22</v>
       </c>
+      <c r="AB18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2255,10 +2370,10 @@
         <v>21</v>
       </c>
       <c r="X19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z19" t="s">
         <v>22</v>
@@ -2266,8 +2381,14 @@
       <c r="AA19" t="s">
         <v>22</v>
       </c>
+      <c r="AB19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2338,10 +2459,10 @@
         <v>21</v>
       </c>
       <c r="X20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z20" t="s">
         <v>22</v>
@@ -2349,8 +2470,14 @@
       <c r="AA20" t="s">
         <v>22</v>
       </c>
+      <c r="AB20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2421,10 +2548,10 @@
         <v>21</v>
       </c>
       <c r="X21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z21" t="s">
         <v>22</v>
@@ -2432,8 +2559,14 @@
       <c r="AA21" t="s">
         <v>22</v>
       </c>
+      <c r="AB21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2504,10 +2637,10 @@
         <v>21</v>
       </c>
       <c r="X22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z22" t="s">
         <v>22</v>
@@ -2515,8 +2648,14 @@
       <c r="AA22" t="s">
         <v>22</v>
       </c>
+      <c r="AB22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2587,10 +2726,10 @@
         <v>21</v>
       </c>
       <c r="X23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z23" t="s">
         <v>22</v>
@@ -2598,8 +2737,14 @@
       <c r="AA23" t="s">
         <v>22</v>
       </c>
+      <c r="AB23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2670,10 +2815,10 @@
         <v>21</v>
       </c>
       <c r="X24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z24" t="s">
         <v>22</v>
@@ -2681,8 +2826,14 @@
       <c r="AA24" t="s">
         <v>22</v>
       </c>
+      <c r="AB24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2753,10 +2904,10 @@
         <v>21</v>
       </c>
       <c r="X25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z25" t="s">
         <v>22</v>
@@ -2764,8 +2915,14 @@
       <c r="AA25" t="s">
         <v>22</v>
       </c>
+      <c r="AB25" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2836,10 +2993,10 @@
         <v>21</v>
       </c>
       <c r="X26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z26" t="s">
         <v>22</v>
@@ -2847,8 +3004,14 @@
       <c r="AA26" t="s">
         <v>22</v>
       </c>
+      <c r="AB26" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2919,10 +3082,10 @@
         <v>21</v>
       </c>
       <c r="X27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z27" t="s">
         <v>22</v>
@@ -2930,8 +3093,14 @@
       <c r="AA27" t="s">
         <v>22</v>
       </c>
+      <c r="AB27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2999,10 +3168,10 @@
         <v>21</v>
       </c>
       <c r="W28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y28" t="s">
         <v>22</v>
@@ -3013,8 +3182,14 @@
       <c r="AA28" t="s">
         <v>22</v>
       </c>
+      <c r="AB28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -3091,13 +3266,19 @@
         <v>21</v>
       </c>
       <c r="Z29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA29" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -3174,13 +3355,19 @@
         <v>21</v>
       </c>
       <c r="Z30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA30" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -3257,13 +3444,19 @@
         <v>21</v>
       </c>
       <c r="Z31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA31" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -3340,13 +3533,19 @@
         <v>21</v>
       </c>
       <c r="Z32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA32" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -3423,13 +3622,19 @@
         <v>21</v>
       </c>
       <c r="Z33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA33" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -3506,13 +3711,19 @@
         <v>21</v>
       </c>
       <c r="Z34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA34" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -3589,13 +3800,19 @@
         <v>21</v>
       </c>
       <c r="Z35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA35" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -3672,13 +3889,19 @@
         <v>21</v>
       </c>
       <c r="Z36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -3755,13 +3978,19 @@
         <v>21</v>
       </c>
       <c r="Z37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA37" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -3838,13 +4067,19 @@
         <v>21</v>
       </c>
       <c r="Z38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA38" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -3921,13 +4156,19 @@
         <v>21</v>
       </c>
       <c r="Z39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -4004,13 +4245,19 @@
         <v>21</v>
       </c>
       <c r="Z40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -4092,8 +4339,14 @@
       <c r="AA41" t="s">
         <v>21</v>
       </c>
+      <c r="AB41" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -4175,8 +4428,14 @@
       <c r="AA42" t="s">
         <v>21</v>
       </c>
+      <c r="AB42" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -4258,8 +4517,14 @@
       <c r="AA43" t="s">
         <v>21</v>
       </c>
+      <c r="AB43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
@@ -4341,8 +4606,14 @@
       <c r="AA44" t="s">
         <v>21</v>
       </c>
+      <c r="AB44" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -4424,8 +4695,14 @@
       <c r="AA45" t="s">
         <v>21</v>
       </c>
+      <c r="AB45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -4507,8 +4784,14 @@
       <c r="AA46" t="s">
         <v>21</v>
       </c>
+      <c r="AB46" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -4590,8 +4873,14 @@
       <c r="AA47" t="s">
         <v>21</v>
       </c>
+      <c r="AB47" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
@@ -4673,8 +4962,14 @@
       <c r="AA48" t="s">
         <v>21</v>
       </c>
+      <c r="AB48" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>57</v>
       </c>
@@ -4754,6 +5049,12 @@
         <v>21</v>
       </c>
       <c r="AA49" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC49" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>